<commit_message>
clone graph problem solved
</commit_message>
<xml_diff>
--- a/graph-leetcode-que/graph_questions_faang.xlsx
+++ b/graph-leetcode-que/graph_questions_faang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Genome\Python\graph-leetcode-que\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60C2401A-CAC2-47C2-9700-A645CEED5993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454F2040-650A-49DE-A993-EF88515C35D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7341DA10-11EE-4FA9-B316-F6D17BA48768}"/>
   </bookViews>
@@ -690,6 +690,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10E52193-0D44-47EA-9434-B098BDA877EB}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0">
+  <autoFilter ref="A1:D32" xr:uid="{10E52193-0D44-47EA-9434-B098BDA877EB}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{88989F2B-B915-4AE6-84DD-CA43C79610DB}" name="Category"/>
+    <tableColumn id="2" xr3:uid="{356ACD3F-9E12-4C23-BFE1-DDEDE6673EE9}" name="Problem"/>
+    <tableColumn id="3" xr3:uid="{47641DEA-B61A-4BE9-AEAB-FC4B77BCB30C}" name="LeetCode #"/>
+    <tableColumn id="4" xr3:uid="{5C463B5E-B891-4ADD-8F27-2B36F58CF508}" name="Difficulty"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -992,15 +1005,15 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1452,6 +1465,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Question status" prompt="Completed" sqref="D2" xr:uid="{2A7674D8-3D43-4DF3-91BE-7855BBC1B738}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
max number of islands problem solved
</commit_message>
<xml_diff>
--- a/graph-leetcode-que/graph_questions_faang.xlsx
+++ b/graph-leetcode-que/graph_questions_faang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Genome\Python\graph-leetcode-que\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454F2040-650A-49DE-A993-EF88515C35D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F130A91F-FD63-432C-81B7-7F18C2D8CAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7341DA10-11EE-4FA9-B316-F6D17BA48768}"/>
   </bookViews>
@@ -1005,7 +1005,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,8 +1465,9 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Question status" prompt="Completed" sqref="D2" xr:uid="{2A7674D8-3D43-4DF3-91BE-7855BBC1B738}"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Question Status" prompt="Completed" sqref="D2" xr:uid="{2A7674D8-3D43-4DF3-91BE-7855BBC1B738}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Question Status" prompt="Completed" sqref="D3" xr:uid="{23486BEB-35E9-4252-8DAE-D0594FE0312E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
flood fill problem solved
</commit_message>
<xml_diff>
--- a/graph-leetcode-que/graph_questions_faang.xlsx
+++ b/graph-leetcode-que/graph_questions_faang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Genome\Python\graph-leetcode-que\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F130A91F-FD63-432C-81B7-7F18C2D8CAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0C93A1-983D-456B-BDD5-82AD6AC3D060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7341DA10-11EE-4FA9-B316-F6D17BA48768}"/>
   </bookViews>
@@ -1005,7 +1005,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,9 +1465,8 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Question Status" prompt="Completed" sqref="D2" xr:uid="{2A7674D8-3D43-4DF3-91BE-7855BBC1B738}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Question Status" prompt="Completed" sqref="D3" xr:uid="{23486BEB-35E9-4252-8DAE-D0594FE0312E}"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Question Status" prompt="Completed" sqref="D2:D3 D4" xr:uid="{2A7674D8-3D43-4DF3-91BE-7855BBC1B738}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>